<commit_message>
Kuisen van de repository, updaten van logboek en componenten lijst
</commit_message>
<xml_diff>
--- a/Algemene documentatie/Logboek.xlsx
+++ b/Algemene documentatie/Logboek.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\OneDrive\KU_Leuven\BachlorProef\BachlorProefCommunicatieEnEinde\Algemene documentatie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9fe58f1971da5aea/KU_Leuven/BachlorProef/BachlorProefCommunicatieEnEinde/Algemene documentatie/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5D9016-DAD9-43B6-B42D-314C12252779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{5A5D9016-DAD9-43B6-B42D-314C12252779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CAD2A3B8-EA03-41C9-87D0-404DFA4CAAA9}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="10044" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>TFT lcd schakeling gemaakt en beginnen met uitzoeken hoe het werkt. Het is gelukt om demo projecten up te loaden.</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>Vandaag zijn de componenten toegekomen, en dus heb ik veel vooruitgang kunnen maken! De speciale druk knoppen ontbraken, en er ontbrak ook één keypad. Maar vandaag heb ik met een keypad, een lcd scherm en een solenoïde een werkende breadbord implementatie kunnen maken van het deurslot. De start en reset knop heb ik geschakelt, maar ze hebben nog niet de juiste functionaliteit in de code.</t>
+  </si>
+  <si>
+    <t>6u30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">De timer werkt perfect samen met de andere code, (ik heb timer interrupt hiervoor moeten gebruiken). En ik heb ook de start en reset knop hun gewenste functie kunnen geven (ook via interrupts). Het versturen van het reset signaal is ook klaar. </t>
   </si>
 </sst>
 </file>
@@ -458,7 +464,7 @@
   <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E14:E16"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -530,10 +536,16 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="2"/>
+    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
+        <v>44642</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>

</xml_diff>